<commit_message>
updated text and topics
</commit_message>
<xml_diff>
--- a/Topics.xlsx
+++ b/Topics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annguyen\Desktop\School\IBS-Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0F99D76-8C59-48DB-8398-A339A21A9F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85B35F3-0F78-4903-9116-6787FA445FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{1EAD38B9-1105-4072-A829-3FA592DB7D9D}"/>
+    <workbookView xWindow="1530" yWindow="3135" windowWidth="21600" windowHeight="11295" xr2:uid="{1EAD38B9-1105-4072-A829-3FA592DB7D9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 30 words" sheetId="1" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>Topic 7</t>
   </si>
   <si>
-    <t>Topic 8</t>
-  </si>
-  <si>
     <t>representation</t>
   </si>
   <si>
@@ -621,6 +618,9 @@
   </si>
   <si>
     <t>regularly</t>
+  </si>
+  <si>
+    <t>Topic 0</t>
   </si>
 </sst>
 </file>
@@ -1020,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12821C37-6C3C-4246-9C40-E952759447F7}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H31" sqref="A1:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,28 +1037,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1066,25 +1066,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1092,25 +1092,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1118,25 +1118,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1144,25 +1144,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1170,25 +1170,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1196,25 +1196,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1222,25 +1222,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1248,25 +1248,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1274,25 +1274,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1300,25 +1300,25 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1326,25 +1326,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1352,25 +1352,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1378,25 +1378,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1404,25 +1404,25 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1430,25 +1430,25 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1456,25 +1456,25 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1482,25 +1482,25 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1508,25 +1508,25 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1534,25 +1534,25 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1560,25 +1560,25 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1586,25 +1586,25 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1612,25 +1612,25 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1638,25 +1638,25 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1664,25 +1664,25 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1693,22 +1693,22 @@
         <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1716,25 +1716,25 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1742,25 +1742,25 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1768,25 +1768,25 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1794,51 +1794,51 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>